<commit_message>
Priority reasoning + Made sec doc
</commit_message>
<xml_diff>
--- a/TemplateForSD6503.xlsx
+++ b/TemplateForSD6503.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w2shared-my.sharepoint.com/personal/richa_panjabi_weltec_ac_nz/Documents/WelTec Trimester 2 2024/SD6503/Assignments/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w2shared-my.sharepoint.com/personal/dave_sushames01_student_wandw_ac_nz/Documents/Documents/Testing and Secure Coding/GroupAssignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{1C52F858-5A85-4961-B84A-0D2BE88D792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10ABB1A1-378D-43C9-B0EE-184C0992E004}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{1C52F858-5A85-4961-B84A-0D2BE88D792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D20B2E40-8360-44A8-B9AC-F32F596E48B5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84DD0BDD-34A0-4121-B413-A041E4D23E14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84DD0BDD-34A0-4121-B413-A041E4D23E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,15 +430,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1181330</xdr:colOff>
+      <xdr:colOff>1209905</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>129541</xdr:rowOff>
+      <xdr:rowOff>120016</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -468,8 +468,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4572001" y="9324976"/>
-          <a:ext cx="2972029" cy="1314450"/>
+          <a:off x="4600576" y="7486651"/>
+          <a:ext cx="2972029" cy="1320165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -964,31 +964,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B856E9-6BC2-4688-8551-28BD4218AC9B}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" customWidth="1"/>
-    <col min="5" max="5" width="39.88671875" customWidth="1"/>
-    <col min="6" max="6" width="43.44140625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="49.44140625" customWidth="1"/>
-    <col min="10" max="10" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="49.42578125" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9"/>
       <c r="C5" s="1"/>
@@ -1034,13 +1034,13 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="55.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
@@ -1096,13 +1096,13 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="C13" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
@@ -1110,7 +1110,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1118,38 +1118,38 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="I21" s="10"/>
     </row>
-    <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="C32" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>27</v>
       </c>

</xml_diff>